<commit_message>
Fixed error in F
</commit_message>
<xml_diff>
--- a/Convergence_Analisys.xlsx
+++ b/Convergence_Analisys.xlsx
@@ -480,7 +480,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -491,7 +491,7 @@
   <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -550,7 +550,7 @@
         <v>6.2500000000000001E-5</v>
       </c>
       <c r="F3" s="5">
-        <f t="shared" ref="F3:G3" si="0">E3/4</f>
+        <f t="shared" ref="F3" si="0">E3/4</f>
         <v>1.5625E-5</v>
       </c>
       <c r="G3" s="5">
@@ -566,20 +566,12 @@
         <v>0.02</v>
       </c>
       <c r="C4" s="6">
-        <v>4.3385339190556202E-5</v>
-      </c>
-      <c r="D4" s="7">
-        <v>4.1270315908298798E-5</v>
-      </c>
-      <c r="E4" s="7">
-        <v>4.0731740836077997E-5</v>
-      </c>
-      <c r="F4" s="7">
-        <v>4.0596472500093497E-5</v>
-      </c>
-      <c r="G4" s="7">
-        <v>4.0562616210695401E-5</v>
-      </c>
+        <v>5.4757800416800498E-5</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="3">
@@ -589,21 +581,13 @@
         <f t="shared" ref="B5:B8" si="1">1/A5</f>
         <v>0.01</v>
       </c>
-      <c r="C5" s="7">
-        <v>4.3074140031653497E-5</v>
-      </c>
+      <c r="C5" s="7"/>
       <c r="D5" s="6">
-        <v>4.1021050638800003E-5</v>
-      </c>
-      <c r="E5" s="7">
-        <v>4.0497732165471502E-5</v>
-      </c>
-      <c r="F5" s="10">
-        <v>4.0366261350217597E-5</v>
-      </c>
-      <c r="G5" s="7">
-        <v>4.0333353362231899E-5</v>
-      </c>
+        <v>4.4107795764842201E-5</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="3">
@@ -613,21 +597,13 @@
         <f t="shared" si="1"/>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C6" s="7">
-        <v>4.1899046072988503E-5</v>
-      </c>
-      <c r="D6" s="7">
-        <v>3.9865505176878003E-5</v>
-      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
       <c r="E6" s="6">
-        <v>3.9346915833307201E-5</v>
-      </c>
-      <c r="F6" s="11">
-        <v>3.92166167162335E-5</v>
-      </c>
-      <c r="G6" s="11">
-        <v>3.9184000979869502E-5</v>
-      </c>
+        <v>4.0093271230321599E-5</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="3">
@@ -637,21 +613,13 @@
         <f t="shared" si="1"/>
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="C7" s="7">
-        <v>4.1221011436600897E-5</v>
-      </c>
-      <c r="D7" s="7">
-        <v>3.9196610214754102E-5</v>
-      </c>
-      <c r="E7" s="7">
-        <v>3.8680245876903401E-5</v>
-      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
       <c r="F7" s="9">
-        <v>3.8550499025490603E-5</v>
-      </c>
-      <c r="G7" s="11">
-        <v>3.8518021102488903E-5</v>
-      </c>
+        <v>3.8696697953271198E-5</v>
+      </c>
+      <c r="G7" s="11"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="3">
@@ -661,20 +629,12 @@
         <f t="shared" si="1"/>
         <v>1.25E-3</v>
       </c>
-      <c r="C8" s="7">
-        <v>4.0902561460213502E-5</v>
-      </c>
-      <c r="D8" s="7">
-        <v>3.8887007830713998E-5</v>
-      </c>
-      <c r="E8" s="7">
-        <v>3.8372855079404199E-5</v>
-      </c>
-      <c r="F8" s="11">
-        <v>3.8243661031496399E-5</v>
-      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="11"/>
       <c r="G8" s="9">
-        <v>3.8211321302271902E-5</v>
+        <v>3.8225804485871197E-5</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -756,7 +716,7 @@
       <c r="C15" s="7"/>
       <c r="D15" s="6">
         <f>C4/D5</f>
-        <v>1.0576359823782748</v>
+        <v>1.2414540211607512</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
@@ -774,7 +734,7 @@
       <c r="D16" s="7"/>
       <c r="E16" s="6">
         <f>D5/E6</f>
-        <v>1.0425480566910317</v>
+        <v>1.1001296330114494</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
@@ -792,7 +752,7 @@
       <c r="E17" s="7"/>
       <c r="F17" s="6">
         <f>E6/F7</f>
-        <v>1.0206590531367696</v>
+        <v>1.0360902441530504</v>
       </c>
       <c r="G17" s="7"/>
     </row>
@@ -810,7 +770,7 @@
       <c r="F18" s="7"/>
       <c r="G18" s="6">
         <f>F7/G8</f>
-        <v>1.0088763673084118</v>
+        <v>1.0123187326920497</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -892,7 +852,7 @@
       <c r="C25" s="7"/>
       <c r="D25" s="6">
         <f>LOG(D15,2)</f>
-        <v>8.0843165463944697E-2</v>
+        <v>0.31203083044610547</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
@@ -910,7 +870,7 @@
       <c r="D26" s="7"/>
       <c r="E26" s="6">
         <f>LOG(E16,2)</f>
-        <v>6.0113886837213866E-2</v>
+        <v>0.13767353273500912</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
@@ -928,7 +888,7 @@
       <c r="E27" s="7"/>
       <c r="F27" s="6">
         <f>LOG(F17,2)</f>
-        <v>2.9501020480888342E-2</v>
+        <v>5.1149668200030245E-2</v>
       </c>
       <c r="G27" s="7"/>
     </row>
@@ -946,7 +906,7 @@
       <c r="F28" s="7"/>
       <c r="G28" s="6">
         <f>LOG(G18,2)</f>
-        <v>1.2749390302130546E-2</v>
+        <v>1.766359998901312E-2</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1025,17 +985,17 @@
         <f t="shared" ref="B40:B43" si="10">1/A40</f>
         <v>0.01</v>
       </c>
-      <c r="C40" s="7">
+      <c r="C40" s="7" t="e">
         <f>C4/C5</f>
-        <v>1.0072247329528579</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D40" s="7">
         <f t="shared" ref="D40:E40" si="11">D4/D5</f>
-        <v>1.0060765208500786</v>
-      </c>
-      <c r="E40" s="7">
+        <v>0</v>
+      </c>
+      <c r="E40" s="7" t="e">
         <f t="shared" si="11"/>
-        <v>1.0057783154288824</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F40" s="7"/>
       <c r="G40" s="7"/>
@@ -1048,21 +1008,21 @@
         <f t="shared" si="10"/>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C41" s="7">
+      <c r="C41" s="7" t="e">
         <f t="shared" ref="C41:F41" si="12">C5/C6</f>
-        <v>1.0280458403902077</v>
-      </c>
-      <c r="D41" s="7">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D41" s="7" t="e">
         <f t="shared" si="12"/>
-        <v>1.0289860985529971</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E41" s="7">
         <f t="shared" si="12"/>
-        <v>1.0292479425081174</v>
-      </c>
-      <c r="F41" s="7">
+        <v>0</v>
+      </c>
+      <c r="F41" s="7" t="e">
         <f t="shared" si="12"/>
-        <v>1.02931524262541</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="G41" s="7"/>
     </row>
@@ -1074,25 +1034,25 @@
         <f t="shared" si="10"/>
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="C42" s="7">
+      <c r="C42" s="7" t="e">
         <f t="shared" ref="C42:G42" si="13">C6/C7</f>
-        <v>1.0164487627245742</v>
-      </c>
-      <c r="D42" s="7">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D42" s="7" t="e">
         <f t="shared" si="13"/>
-        <v>1.017065122684311</v>
-      </c>
-      <c r="E42" s="7">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E42" s="7" t="e">
         <f t="shared" si="13"/>
-        <v>1.0172354115463853</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F42" s="7">
         <f t="shared" si="13"/>
-        <v>1.0172790938530378</v>
-      </c>
-      <c r="G42" s="7">
+        <v>0</v>
+      </c>
+      <c r="G42" s="7" t="e">
         <f t="shared" si="13"/>
-        <v>1.0172900854799511</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1103,25 +1063,25 @@
         <f t="shared" si="10"/>
         <v>1.25E-3</v>
       </c>
-      <c r="C43" s="7">
+      <c r="C43" s="7" t="e">
         <f t="shared" ref="C43:G43" si="14">C7/C8</f>
-        <v>1.007785575402097</v>
-      </c>
-      <c r="D43" s="7">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D43" s="7" t="e">
         <f t="shared" si="14"/>
-        <v>1.0079615892636402</v>
-      </c>
-      <c r="E43" s="7">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E43" s="7" t="e">
         <f t="shared" si="14"/>
-        <v>1.0080106313919859</v>
-      </c>
-      <c r="F43" s="7">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F43" s="7" t="e">
         <f t="shared" si="14"/>
-        <v>1.0080232379881597</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="G43" s="7">
         <f t="shared" si="14"/>
-        <v>1.0080264118005982</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -1200,17 +1160,17 @@
         <f t="shared" ref="B50:B53" si="17">1/A50</f>
         <v>0.01</v>
       </c>
-      <c r="C50" s="7">
+      <c r="C50" s="7" t="e">
         <f>LOG(C40,2)</f>
-        <v>1.0385614768389778E-2</v>
-      </c>
-      <c r="D50" s="7">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D50" s="7" t="e">
         <f t="shared" ref="D50:E50" si="18">LOG(D40,2)</f>
-        <v>8.7400387940663928E-3</v>
-      </c>
-      <c r="E50" s="7">
+        <v>#NUM!</v>
+      </c>
+      <c r="E50" s="7" t="e">
         <f t="shared" si="18"/>
-        <v>8.3123543729852461E-3</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>
@@ -1223,21 +1183,21 @@
         <f t="shared" si="17"/>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C51" s="7">
+      <c r="C51" s="7" t="e">
         <f t="shared" ref="C51:F51" si="19">LOG(C41,2)</f>
-        <v>3.9904595494006899E-2</v>
-      </c>
-      <c r="D51" s="7">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D51" s="7" t="e">
         <f t="shared" si="19"/>
-        <v>4.1223491771118156E-2</v>
-      </c>
-      <c r="E51" s="7">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E51" s="7" t="e">
         <f t="shared" si="19"/>
-        <v>4.1590564679291411E-2</v>
-      </c>
-      <c r="F51" s="7">
+        <v>#NUM!</v>
+      </c>
+      <c r="F51" s="7" t="e">
         <f t="shared" si="19"/>
-        <v>4.1684896051974139E-2</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="G51" s="7"/>
     </row>
@@ -1249,25 +1209,25 @@
         <f t="shared" si="17"/>
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="C52" s="7">
+      <c r="C52" s="7" t="e">
         <f t="shared" ref="C52:G52" si="20">LOG(C42,2)</f>
-        <v>2.3537493464777733E-2</v>
-      </c>
-      <c r="D52" s="7">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D52" s="7" t="e">
         <f t="shared" si="20"/>
-        <v>2.4412057922808966E-2</v>
-      </c>
-      <c r="E52" s="7">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E52" s="7" t="e">
         <f t="shared" si="20"/>
-        <v>2.4653590472472182E-2</v>
-      </c>
-      <c r="F52" s="7">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F52" s="7" t="e">
         <f t="shared" si="20"/>
-        <v>2.4715541613173929E-2</v>
-      </c>
-      <c r="G52" s="7">
+        <v>#NUM!</v>
+      </c>
+      <c r="G52" s="7" t="e">
         <f t="shared" si="20"/>
-        <v>2.4731129744361972E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -1278,25 +1238,25 @@
         <f t="shared" si="17"/>
         <v>1.25E-3</v>
       </c>
-      <c r="C53" s="9">
+      <c r="C53" s="9" t="e">
         <f t="shared" ref="C53:G53" si="21">LOG(C43,2)</f>
-        <v>1.1188712040673114E-2</v>
-      </c>
-      <c r="D53" s="7">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D53" s="7" t="e">
         <f t="shared" si="21"/>
-        <v>1.1440662612920195E-2</v>
-      </c>
-      <c r="E53" s="7">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E53" s="7" t="e">
         <f t="shared" si="21"/>
-        <v>1.1510854885063588E-2</v>
-      </c>
-      <c r="F53" s="7">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F53" s="7" t="e">
         <f t="shared" si="21"/>
-        <v>1.1528897710691656E-2</v>
-      </c>
-      <c r="G53" s="7">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G53" s="7" t="e">
         <f t="shared" si="21"/>
-        <v>1.1533440102260336E-2</v>
+        <v>#NUM!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>